<commit_message>
Events And Notices Display Added
</commit_message>
<xml_diff>
--- a/public/school_sample_data.xlsx
+++ b/public/school_sample_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pranavsharma/Desktop/Events/SIH/SIH-Upasthiti/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B801EDD7-B4FE-994F-979D-4E2E19C6186B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA281F3-2925-F74C-9311-63697ED4F46E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17540" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17540" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2372" uniqueCount="732">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2375" uniqueCount="732">
   <si>
     <t>Class ID</t>
   </si>
@@ -10757,10 +10757,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10771,7 +10771,7 @@
     <col min="4" max="4" width="22.5" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>708</v>
       </c>
@@ -10784,8 +10784,11 @@
       <c r="D1" s="1" t="s">
         <v>710</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>711</v>
       </c>
@@ -10798,8 +10801,11 @@
       <c r="D2" s="2" t="s">
         <v>713</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="2" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>714</v>
       </c>
@@ -10812,6 +10818,45 @@
       <c r="D3" s="2" t="s">
         <v>717</v>
       </c>
+      <c r="E3" s="2" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -10823,7 +10868,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="E1" sqref="E1:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10895,7 +10940,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65026444-F0CD-5047-B980-7E3E6FA9E306}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>

</xml_diff>